<commit_message>
corsConfiguration - Config Class commit
</commit_message>
<xml_diff>
--- a/Schema_Description.xlsx
+++ b/Schema_Description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HealthEcho\HealthEcho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HealthEcho-BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3847298-F47B-4A23-A800-0DEEB6ABA8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D3D07F-3A37-4A64-B54F-39C04E094218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A7DB545-7496-46AF-9D9B-B1D0D5ECA28D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>column_name</t>
   </si>
@@ -96,12 +96,6 @@
     <t>symptom</t>
   </si>
   <si>
-    <t>vital_signs</t>
-  </si>
-  <si>
-    <t>jsonb</t>
-  </si>
-  <si>
     <t>health_logs</t>
   </si>
   <si>
@@ -118,6 +112,24 @@
   </si>
   <si>
     <t>HealthEcho Table Description</t>
+  </si>
+  <si>
+    <t>blood_glucose</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>blood_pressure</t>
+  </si>
+  <si>
+    <t>oxygen_saturation</t>
+  </si>
+  <si>
+    <t>pulse_rate</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -507,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E120033-51C2-4833-A01B-33DBBC7EDF17}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="105" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,7 +533,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4"/>
     </row>
@@ -597,7 +609,7 @@
     </row>
     <row r="16" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3"/>
     </row>
@@ -683,63 +695,87 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
         <v>8</v>
       </c>
     </row>
@@ -747,7 +783,7 @@
   <mergeCells count="4">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>